<commit_message>
Adiciona nova planilha de saída
</commit_message>
<xml_diff>
--- a/dados/horarios_2024_teste.xlsx
+++ b/dados/horarios_2024_teste.xlsx
@@ -55,25 +55,35 @@
       <style:table-row-properties style:row-height="0.919cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro3" style:family="table-row">
-      <style:table-row-properties style:row-height="0.452cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="0.471cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro4" style:family="table-row">
       <style:table-row-properties style:row-height="1.002cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro5" style:family="table-row">
+      <style:table-row-properties style:row-height="0.452cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    </style:style>
+    <style:style style:name="ro6" style:family="table-row">
       <style:table-row-properties style:row-height="0.841cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
-    <style:style style:name="ro6" style:family="table-row">
+    <style:style style:name="ro7" style:family="table-row">
       <style:table-row-properties style:row-height="1.632cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
-    <style:style style:name="ro7" style:family="table-row">
+    <style:style style:name="ro8" style:family="table-row">
       <style:table-row-properties style:row-height="2.422cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
-    <style:style style:name="ro8" style:family="table-row">
+    <style:style style:name="ro9" style:family="table-row">
       <style:table-row-properties style:row-height="1.236cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
+    </style:style>
+    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="transparent" fo:wrap-option="wrap"/>
+      <style:text-properties fo:font-weight="normal" style:font-weight-asian="normal" style:font-weight-complex="normal"/>
+    </style:style>
+    <style:style style:name="ce19" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="transparent" fo:wrap-option="wrap"/>
     </style:style>
     <style:style style:name="ce23" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:wrap-option="wrap"/>
@@ -81,9 +91,6 @@
     </style:style>
     <style:style style:name="ce24" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:wrap-option="wrap"/>
-    </style:style>
-    <style:style style:name="ce19" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="transparent" fo:wrap-option="wrap"/>
     </style:style>
     <style:style style:name="ce25" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" style:vertical-align="middle"/>
@@ -123,7 +130,7 @@
         <table:table-column table:style-name="co4" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co5" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co6" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co7" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co7" table:default-cell-style-name="ce19"/>
         <table:table-column table:style-name="co8" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -144,7 +151,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>horario</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+            <text:p>vagas</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -169,7 +179,10 @@
               2T45 (10/06/2024 - 15/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -194,7 +207,10 @@
               2T45 (10/06/2024 - 15/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -219,7 +235,10 @@
               4T45 (17/06/2024 - 22/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -244,7 +263,10 @@
               2T12 (10/06/2024 - 15/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -269,7 +291,10 @@
               2T12 (10/06/2024 - 15/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -294,7 +319,10 @@
               6T45 (17/06/2024 - 22/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -319,7 +347,10 @@
               6T12 (17/06/2024 - 22/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -340,7 +371,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>3N1234 (04/03/2024 - 06/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -361,7 +395,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>5N1234 (04/03/2024 - 13/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -382,7 +419,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>2N1234 (04/03/2024 - 06/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -403,7 +443,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>2N1234 (04/03/2024 - 06/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -424,7 +467,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>4N1234 (04/03/2024 - 13/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -445,7 +491,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>6N1234 (04/03/2024 - 13/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="60" calcext:value-type="float">
+            <text:p>60</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -470,7 +519,10 @@
               3T12 (08/07/2024 - 13/07/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="55" calcext:value-type="float">
+            <text:p>55</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -491,7 +543,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>2T45 4T123 (04/03/2024 - 15/06/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -516,7 +571,10 @@
               5T45 (17/06/2024 - 22/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="30" calcext:value-type="float">
+            <text:p>30</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -541,7 +599,10 @@
               5T45 (17/06/2024 - 22/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -566,7 +627,10 @@
               2T12 (10/06/2024 - 15/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -591,7 +655,10 @@
               2T12 (10/06/2024 - 15/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -612,7 +679,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>5N1234 (04/03/2024 - 13/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -633,7 +703,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>2N1234 (04/03/2024 - 06/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -654,7 +727,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>6N1234 (04/03/2024 - 13/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -675,7 +751,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>4N1234 (04/03/2024 - 13/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -696,7 +775,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>3N1234 (04/03/2024 - 06/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -717,7 +799,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>3N1234 (04/03/2024 - 06/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -742,7 +827,10 @@
               5T12 (17/06/2024 - 22/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -767,7 +855,10 @@
               3T45 (10/06/2024 - 15/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -792,7 +883,10 @@
               6T45 (17/06/2024 - 22/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -817,7 +911,10 @@
               3T12 (10/06/2024 - 15/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -842,7 +939,10 @@
               6T12 (17/06/2024 - 22/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -863,7 +963,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>5N1234 (04/03/2024 - 13/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -884,7 +987,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>4N1234 (04/03/2024 - 13/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -905,7 +1011,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>6N1234 (04/03/2024 - 13/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -926,7 +1035,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>3N1234 (04/03/2024 - 06/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -947,7 +1059,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>2N1234 (04/03/2024 - 06/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro4">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -968,7 +1083,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>2T45 4T123 (04/03/2024 - 15/06/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -989,7 +1107,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>3N1234 (04/03/2024 - 06/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1010,7 +1131,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>3T45 6T123 (04/03/2024 - 15/06/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1035,7 +1159,10 @@
               2T12 6T45 (10/06/2024 - 15/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1060,7 +1187,10 @@
               4T12 (17/06/2024 - 22/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1081,7 +1211,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>6N1234 (04/03/2024 - 13/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="40" calcext:value-type="float">
+            <text:p>40</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1102,7 +1235,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>3N1234 (04/03/2024 - 06/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="40" calcext:value-type="float">
+            <text:p>40</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1123,7 +1259,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>2N1234 (04/03/2024 - 06/07/2024)</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="40" calcext:value-type="float">
+            <text:p>40</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1148,7 +1287,10 @@
               7T1 (04/03/2024 - 06/07/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="40" calcext:value-type="float">
+            <text:p>40</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1173,7 +1315,10 @@
               7T123456 (04/03/2024 - 15/06/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="40" calcext:value-type="float">
+            <text:p>40</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1198,7 +1343,10 @@
               7T123456 (04/03/2024 - 06/07/2024)
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
       </table:table>
       <table:table table:name="Turmas Divididas" table:style-name="ta1">
@@ -1206,7 +1354,7 @@
         <table:table-column table:style-name="co9" table:default-cell-style-name="ce25"/>
         <table:table-column table:style-name="co9" table:number-columns-repeated="1008" table:default-cell-style-name="ce19"/>
         <table:table-column table:style-name="co9" table:default-cell-style-name="ce20"/>
-        <table:table-row table:style-name="ro5">
+        <table:table-row table:style-name="ro6">
           <table:table-cell table:style-name="ce23" office:value-type="string" calcext:value-type="string">
             <text:p>ano</text:p>
           </table:table-cell>
@@ -1254,100 +1402,6 @@
           </table:table-cell>
           <table:table-cell table:style-name="ce18" table:number-columns-repeated="1008"/>
           <table:table-cell table:style-name="ce14"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro6">
-          <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
-            <text:p>2024</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
-            <text:p>1</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1501" calcext:value-type="float">
-            <text:p>1501</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>AGRONOMIA</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>GCB0602</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>MORFOLOGIA VEGETAL</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="45" calcext:value-type="float">
-            <text:p>45</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="51876" calcext:value-type="float">
-            <text:p>51876</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
-            <text:p>1</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>6M34 (04/03/2024 - 13/07/2024)</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
-            <text:p>50</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>ROSIANE BERENICE NICOLOSO DENARDIN</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="30" calcext:value-type="float">
-            <text:p>30</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>ABERTA</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="100" calcext:value-type="float" table:number-columns-spanned="1" table:number-rows-spanned="2">
-            <text:p>100</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1009"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro6">
-          <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
-            <text:p>2024</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
-            <text:p>1</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1501" calcext:value-type="float">
-            <text:p>1501</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>AGRONOMIA</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>GCB0602</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>MORFOLOGIA VEGETAL</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="45" calcext:value-type="float">
-            <text:p>45</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="51877" calcext:value-type="float">
-            <text:p>51877</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
-            <text:p>1</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>6M35 (04/03/2024 - 13/07/2024)</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="25" calcext:value-type="float">
-            <text:p>25</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>ROSIANE BERENICE NICOLOSO DENARDIN</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="15" calcext:value-type="float">
-            <text:p>15</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>ABERTA</text:p>
-          </table:table-cell>
-          <table:covered-table-cell table:style-name="ce24"/>
-          <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
         <table:table-row table:style-name="ro7">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
@@ -1363,37 +1417,37 @@
             <text:p>AGRONOMIA</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>GEX1104</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>QUÍMICA GERAL E INORGÂNICA</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
-            <text:p>75</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="51863" calcext:value-type="float">
-            <text:p>51863</text:p>
+            <text:p>GCB0602</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>MORFOLOGIA VEGETAL</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="45" calcext:value-type="float">
+            <text:p>45</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="51876" calcext:value-type="float">
+            <text:p>51876</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
             <text:p>1</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>3M45 4M23 (04/03/2024 - 06/07/2024), 3M4 4M2 (08/07/2024 - 13/07/2024)</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="25" calcext:value-type="float">
-            <text:p>25</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>ARLINDO CRISTIANO FELIPPE</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
-            <text:p>75</text:p>
+            <text:p>6M34 (04/03/2024 - 13/07/2024)</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ROSIANE BERENICE NICOLOSO DENARDIN</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="30" calcext:value-type="float">
+            <text:p>30</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>ABERTA</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="101" calcext:value-type="float" table:number-columns-spanned="1" table:number-rows-spanned="2">
-            <text:p>101</text:p>
+          <table:table-cell office:value-type="float" office:value="100" calcext:value-type="float" table:number-columns-spanned="1" table:number-rows-spanned="2">
+            <text:p>100</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
@@ -1411,31 +1465,31 @@
             <text:p>AGRONOMIA</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>GEX1104</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>QUÍMICA GERAL E INORGÂNICA</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
-            <text:p>75</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="51865" calcext:value-type="float">
-            <text:p>51865</text:p>
+            <text:p>GCB0602</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>MORFOLOGIA VEGETAL</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="45" calcext:value-type="float">
+            <text:p>45</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="51877" calcext:value-type="float">
+            <text:p>51877</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
             <text:p>1</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>34M45 (04/03/2024 - 06/07/2024), 34M4 (08/07/2024 - 13/07/2024)</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
-            <text:p>50</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>ARLINDO CRISTIANO FELIPPE</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="30" calcext:value-type="float">
-            <text:p>30</text:p>
+            <text:p>6M35 (04/03/2024 - 13/07/2024)</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="25" calcext:value-type="float">
+            <text:p>25</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ROSIANE BERENICE NICOLOSO DENARDIN</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="15" calcext:value-type="float">
+            <text:p>15</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>ABERTA</text:p>
@@ -1457,6 +1511,100 @@
             <text:p>AGRONOMIA</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>GEX1104</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>QUÍMICA GERAL E INORGÂNICA</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
+            <text:p>75</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="51863" calcext:value-type="float">
+            <text:p>51863</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>3M45 4M23 (04/03/2024 - 06/07/2024), 3M4 4M2 (08/07/2024 - 13/07/2024)</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="25" calcext:value-type="float">
+            <text:p>25</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ARLINDO CRISTIANO FELIPPE</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
+            <text:p>75</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ABERTA</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="101" calcext:value-type="float" table:number-columns-spanned="1" table:number-rows-spanned="2">
+            <text:p>101</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1009"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro8">
+          <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
+            <text:p>2024</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1501" calcext:value-type="float">
+            <text:p>1501</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>AGRONOMIA</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>GEX1104</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>QUÍMICA GERAL E INORGÂNICA</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
+            <text:p>75</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="51865" calcext:value-type="float">
+            <text:p>51865</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>34M45 (04/03/2024 - 06/07/2024), 34M4 (08/07/2024 - 13/07/2024)</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ARLINDO CRISTIANO FELIPPE</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="30" calcext:value-type="float">
+            <text:p>30</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ABERTA</text:p>
+          </table:table-cell>
+          <table:covered-table-cell table:style-name="ce24"/>
+          <table:table-cell table:number-columns-repeated="1009"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro9">
+          <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
+            <text:p>2024</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1501" calcext:value-type="float">
+            <text:p>1501</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>AGRONOMIA</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN081</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1491,7 +1639,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro7">
+        <table:table-row table:style-name="ro8">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -1543,7 +1691,7 @@
           <table:covered-table-cell table:style-name="ce24"/>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro8">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -1591,7 +1739,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro8">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -1637,7 +1785,7 @@
           <table:covered-table-cell table:style-name="ce24"/>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro8">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -1685,7 +1833,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro8">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -1731,7 +1879,7 @@
           <table:covered-table-cell table:style-name="ce24"/>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro7">
+        <table:table-row table:style-name="ro8">
           <table:table-cell table:style-name="ce19" office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -1779,7 +1927,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro7">
+        <table:table-row table:style-name="ro8">
           <table:table-cell table:style-name="ce19" office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -1825,7 +1973,7 @@
           <table:covered-table-cell table:style-name="ce27"/>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro7">
+        <table:table-row table:style-name="ro8">
           <table:table-cell table:style-name="ce19" office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -1873,7 +2021,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro7">
+        <table:table-row table:style-name="ro8">
           <table:table-cell table:style-name="ce19" office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -1939,10 +2087,10 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.2">
   <office:meta>
     <meta:generator>LibreOffice/6.4.7.2$Linux_X86_64 LibreOffice_project/40$Build-2</meta:generator>
-    <dc:date>2024-02-27T10:54:05.706173697</dc:date>
-    <meta:editing-duration>PT2H49M13S</meta:editing-duration>
-    <meta:editing-cycles>27</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="2" meta:cell-count="500" meta:object-count="0"/>
+    <dc:date>2024-04-16T11:13:29.695110228</dc:date>
+    <meta:editing-duration>PT2H49M49S</meta:editing-duration>
+    <meta:editing-cycles>28</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="2" meta:cell-count="547" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -1953,8 +2101,8 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">66583</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">23376</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">80777</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">24230</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
@@ -1978,17 +2126,17 @@
               <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
             </config:config-item-map-entry>
             <config:config-item-map-entry config:name="_WITH_docentes_por_turma_AS_SELECT_dt_id_turma_COALESCE_COUNT_p__202402211025">
-              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">47</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">6</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">45</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">2</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
               <config:config-item config:name="VerticalSplitPosition" config:type="int">1</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
-              <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionLeft" config:type="int">3</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">4</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">1</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">95</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -1997,7 +2145,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">_WITH_docentes_por_turma_AS_SELECT_dt_id_turma_COALESCE_COUNT_p__202402211025</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">900</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1836</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">95</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -2034,7 +2182,7 @@
       <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
       <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">nwH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwAAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpEdXBsZXg6Tm9uZQBQYWdlU2l6ZTpBNAAAEgBDT01QQVRfRFVQTEVYX01PREUPAER1cGxleE1vZGU6Ok9mZg==</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">nwH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwAAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpQYWdlU2l6ZTpBNABEdXBsZXg6Tm9uZQAAEgBDT01QQVRfRFVQTEVYX01PREUPAER1cGxleE1vZGU6Ok9mZg==</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1000</config:config-item>
       <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
@@ -2196,9 +2344,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2024-02-27">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2024-04-16">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="10:48:58.059195813">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="11:12:53.432584105">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>